<commit_message>
Added DBI enable vector
Signed-off-by: Julie Zhang <julie.zhang@intel.com>
</commit_message>
<xml_diff>
--- a/docs/aib_csr_for_2_0_v5.xlsx
+++ b/docs/aib_csr_for_2_0_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huizhan1\open_source\aib-phy-hardware\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F43B90DA-9664-4DE8-ACF1-2AB316414EF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52661B43-0475-4BCB-868F-A6FF0290F935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1305" windowWidth="27045" windowHeight="14325" xr2:uid="{C6002A17-3870-4AD4-B97B-45CCDF04E806}"/>
+    <workbookView xWindow="1050" yWindow="2325" windowWidth="23580" windowHeight="13260" xr2:uid="{C6002A17-3870-4AD4-B97B-45CCDF04E806}"/>
   </bookViews>
   <sheets>
     <sheet name="AIB2.0 Adapt CSR" sheetId="7" r:id="rId1"/>
@@ -2348,9 +2348,6 @@
     <t>11: transmit register mode.</t>
   </si>
   <si>
-    <t>19’b0</t>
-  </si>
-  <si>
     <t>r_tx_dbi_en: transmit DBI (Data Bus Inversion) enable</t>
   </si>
   <si>
@@ -2526,6 +2523,9 @@
   </si>
   <si>
     <t>txswap_en: Only used when in Gen 1 mode for 2xFIFO mode</t>
+  </si>
+  <si>
+    <t>14’b0</t>
   </si>
 </sst>
 </file>
@@ -3334,6 +3334,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3343,41 +3361,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3403,17 +3394,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="4" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3421,10 +3409,22 @@
     <xf numFmtId="22" fontId="4" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3743,8 +3743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490055F6-550E-4468-BB8A-7FE7DCD5F8CF}">
   <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3757,10 +3757,10 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="170" t="s">
-        <v>770</v>
-      </c>
-      <c r="B2" s="170" t="s">
+      <c r="A2" s="176" t="s">
+        <v>769</v>
+      </c>
+      <c r="B2" s="176" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="144" t="s">
@@ -3770,7 +3770,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="161" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F2" s="155" t="s">
         <v>8</v>
@@ -3779,8 +3779,8 @@
       <c r="H2" s="168"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="171"/>
-      <c r="B3" s="171"/>
+      <c r="A3" s="177"/>
+      <c r="B3" s="177"/>
       <c r="C3" s="141" t="s">
         <v>734</v>
       </c>
@@ -3791,13 +3791,13 @@
         <v>731</v>
       </c>
       <c r="F3" s="139" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G3" s="142"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="171"/>
-      <c r="B4" s="171"/>
+      <c r="A4" s="177"/>
+      <c r="B4" s="177"/>
       <c r="C4" s="143"/>
       <c r="D4" s="139"/>
       <c r="E4" s="139"/>
@@ -3807,8 +3807,8 @@
       <c r="G4" s="142"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="171"/>
-      <c r="B5" s="171"/>
+      <c r="A5" s="177"/>
+      <c r="B5" s="177"/>
       <c r="C5" s="143"/>
       <c r="D5" s="139"/>
       <c r="E5" s="139"/>
@@ -3818,8 +3818,8 @@
       <c r="G5" s="142"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="171"/>
-      <c r="B6" s="171"/>
+      <c r="A6" s="177"/>
+      <c r="B6" s="177"/>
       <c r="C6" s="143"/>
       <c r="D6" s="139"/>
       <c r="E6" s="139"/>
@@ -3829,8 +3829,8 @@
       <c r="G6" s="142"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="171"/>
-      <c r="B7" s="171"/>
+      <c r="A7" s="177"/>
+      <c r="B7" s="177"/>
       <c r="C7" s="143"/>
       <c r="D7" s="139"/>
       <c r="E7" s="139"/>
@@ -3840,8 +3840,8 @@
       <c r="G7" s="142"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="171"/>
-      <c r="B8" s="171"/>
+      <c r="A8" s="177"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="143"/>
       <c r="D8" s="139"/>
       <c r="E8" s="139"/>
@@ -3851,8 +3851,8 @@
       <c r="G8" s="142"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="171"/>
-      <c r="B9" s="171"/>
+      <c r="A9" s="177"/>
+      <c r="B9" s="177"/>
       <c r="C9" s="141" t="s">
         <v>735</v>
       </c>
@@ -3868,8 +3868,8 @@
       <c r="G9" s="142"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="171"/>
-      <c r="B10" s="171"/>
+      <c r="A10" s="177"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="144" t="s">
         <v>737</v>
       </c>
@@ -3880,12 +3880,12 @@
         <v>738</v>
       </c>
       <c r="F10" s="139" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="171"/>
-      <c r="B11" s="171"/>
+      <c r="A11" s="177"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="145"/>
       <c r="D11" s="136"/>
       <c r="E11" s="136"/>
@@ -3894,8 +3894,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="171"/>
-      <c r="B12" s="171"/>
+      <c r="A12" s="177"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="146"/>
       <c r="D12" s="137"/>
       <c r="E12" s="137"/>
@@ -3904,51 +3904,51 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="171"/>
-      <c r="B13" s="171"/>
-      <c r="C13" s="194" t="s">
+      <c r="A13" s="177"/>
+      <c r="B13" s="177"/>
+      <c r="C13" s="179" t="s">
         <v>728</v>
       </c>
-      <c r="D13" s="170" t="s">
+      <c r="D13" s="176" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="170" t="s">
+      <c r="E13" s="176" t="s">
         <v>714</v>
       </c>
       <c r="F13" s="128" t="s">
+        <v>815</v>
+      </c>
+      <c r="G13" s="159"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="177"/>
+      <c r="B14" s="177"/>
+      <c r="C14" s="180"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="128" t="s">
         <v>816</v>
       </c>
-      <c r="G13" s="159"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="171"/>
-      <c r="B14" s="171"/>
-      <c r="C14" s="195"/>
-      <c r="D14" s="171"/>
-      <c r="E14" s="171"/>
-      <c r="F14" s="128" t="s">
-        <v>817</v>
-      </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="172"/>
-      <c r="B15" s="172"/>
-      <c r="C15" s="196"/>
-      <c r="D15" s="172"/>
-      <c r="E15" s="172"/>
+      <c r="A15" s="178"/>
+      <c r="B15" s="178"/>
+      <c r="C15" s="181"/>
+      <c r="D15" s="178"/>
+      <c r="E15" s="178"/>
       <c r="F15" s="129" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="170" t="s">
-        <v>771</v>
-      </c>
-      <c r="B16" s="170" t="s">
+      <c r="A16" s="176" t="s">
+        <v>770</v>
+      </c>
+      <c r="B16" s="176" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="131" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D16" s="127" t="s">
         <v>9</v>
@@ -3961,10 +3961,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="171"/>
-      <c r="B17" s="171"/>
+      <c r="A17" s="177"/>
+      <c r="B17" s="177"/>
       <c r="C17" s="144" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="D17" s="155" t="s">
         <v>13</v>
@@ -3973,37 +3973,37 @@
         <v>738</v>
       </c>
       <c r="F17" s="155" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G17" s="169"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="171"/>
-      <c r="B18" s="171"/>
-      <c r="C18" s="197"/>
-      <c r="D18" s="183"/>
-      <c r="E18" s="199"/>
+      <c r="A18" s="177"/>
+      <c r="B18" s="177"/>
+      <c r="C18" s="193"/>
+      <c r="D18" s="173"/>
+      <c r="E18" s="170"/>
       <c r="F18" s="163" t="s">
+        <v>789</v>
+      </c>
+      <c r="G18" s="160"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="177"/>
+      <c r="B19" s="177"/>
+      <c r="C19" s="194"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="171"/>
+      <c r="F19" s="164" t="s">
         <v>790</v>
       </c>
-      <c r="G18" s="160"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="171"/>
-      <c r="B19" s="171"/>
-      <c r="C19" s="198"/>
-      <c r="D19" s="184"/>
-      <c r="E19" s="200"/>
-      <c r="F19" s="164" t="s">
-        <v>791</v>
-      </c>
       <c r="G19" s="160"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="171"/>
-      <c r="B20" s="171"/>
+      <c r="A20" s="177"/>
+      <c r="B20" s="177"/>
       <c r="C20" s="162" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D20" s="126" t="s">
         <v>13</v>
@@ -4012,37 +4012,37 @@
         <v>738</v>
       </c>
       <c r="F20" s="126" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="G20" s="160"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="171"/>
-      <c r="B21" s="171"/>
+      <c r="A21" s="177"/>
+      <c r="B21" s="177"/>
       <c r="C21" s="162"/>
       <c r="D21" s="126"/>
       <c r="E21" s="126"/>
       <c r="F21" s="165" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G21" s="160"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="171"/>
-      <c r="B22" s="171"/>
+      <c r="A22" s="177"/>
+      <c r="B22" s="177"/>
       <c r="C22" s="162"/>
       <c r="D22" s="126"/>
       <c r="E22" s="126"/>
       <c r="F22" s="165" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G22" s="160"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="171"/>
-      <c r="B23" s="171"/>
+      <c r="A23" s="177"/>
+      <c r="B23" s="177"/>
       <c r="C23" s="143" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D23" s="139" t="s">
         <v>13</v>
@@ -4051,37 +4051,37 @@
         <v>738</v>
       </c>
       <c r="F23" s="139" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="G23" s="160"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="171"/>
-      <c r="B24" s="171"/>
+      <c r="A24" s="177"/>
+      <c r="B24" s="177"/>
       <c r="C24" s="145"/>
       <c r="D24" s="156"/>
       <c r="E24" s="156"/>
       <c r="F24" s="167" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G24" s="160"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="171"/>
-      <c r="B25" s="171"/>
+      <c r="A25" s="177"/>
+      <c r="B25" s="177"/>
       <c r="C25" s="146"/>
       <c r="D25" s="157"/>
       <c r="E25" s="126"/>
       <c r="F25" s="166" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G25" s="160"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="171"/>
-      <c r="B26" s="171"/>
+      <c r="A26" s="177"/>
+      <c r="B26" s="177"/>
       <c r="C26" s="144" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D26" s="155" t="s">
         <v>13</v>
@@ -4090,37 +4090,37 @@
         <v>738</v>
       </c>
       <c r="F26" s="139" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G26" s="160"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="171"/>
-      <c r="B27" s="171"/>
+      <c r="A27" s="177"/>
+      <c r="B27" s="177"/>
       <c r="C27" s="162"/>
       <c r="D27" s="126"/>
       <c r="E27" s="156"/>
       <c r="F27" s="167" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="G27" s="160"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="171"/>
-      <c r="B28" s="171"/>
+      <c r="A28" s="177"/>
+      <c r="B28" s="177"/>
       <c r="C28" s="146"/>
       <c r="D28" s="157"/>
       <c r="E28" s="157"/>
       <c r="F28" s="166" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G28" s="160"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="171"/>
-      <c r="B29" s="171"/>
+      <c r="A29" s="177"/>
+      <c r="B29" s="177"/>
       <c r="C29" s="144" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="D29" s="139" t="s">
         <v>13</v>
@@ -4129,42 +4129,42 @@
         <v>738</v>
       </c>
       <c r="F29" s="139" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G29" s="160"/>
     </row>
     <row r="30" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="171"/>
-      <c r="B30" s="171"/>
+      <c r="A30" s="177"/>
+      <c r="B30" s="177"/>
       <c r="C30" s="162"/>
       <c r="D30" s="156"/>
       <c r="E30" s="156"/>
       <c r="F30" s="167" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G30" s="160"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="171"/>
-      <c r="B31" s="171"/>
+      <c r="A31" s="177"/>
+      <c r="B31" s="177"/>
       <c r="C31" s="146"/>
       <c r="D31" s="157"/>
       <c r="E31" s="157"/>
       <c r="F31" s="166" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G31" s="160"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="171"/>
-      <c r="B32" s="171"/>
-      <c r="C32" s="179" t="s">
+      <c r="A32" s="177"/>
+      <c r="B32" s="177"/>
+      <c r="C32" s="190" t="s">
         <v>741</v>
       </c>
-      <c r="D32" s="182" t="s">
+      <c r="D32" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="182" t="s">
+      <c r="E32" s="175" t="s">
         <v>742</v>
       </c>
       <c r="F32" s="148" t="s">
@@ -4172,21 +4172,21 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="171"/>
-      <c r="B33" s="171"/>
-      <c r="C33" s="180"/>
-      <c r="D33" s="183"/>
-      <c r="E33" s="183"/>
+      <c r="A33" s="177"/>
+      <c r="B33" s="177"/>
+      <c r="C33" s="191"/>
+      <c r="D33" s="173"/>
+      <c r="E33" s="173"/>
       <c r="F33" s="148" t="s">
         <v>744</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="171"/>
-      <c r="B34" s="171"/>
-      <c r="C34" s="180"/>
-      <c r="D34" s="183"/>
-      <c r="E34" s="183"/>
+      <c r="A34" s="177"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="191"/>
+      <c r="D34" s="173"/>
+      <c r="E34" s="173"/>
       <c r="F34" s="148" t="s">
         <v>745</v>
       </c>
@@ -4196,11 +4196,11 @@
       <c r="J34" s="147"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="171"/>
-      <c r="B35" s="171"/>
-      <c r="C35" s="180"/>
-      <c r="D35" s="183"/>
-      <c r="E35" s="183"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="177"/>
+      <c r="C35" s="191"/>
+      <c r="D35" s="173"/>
+      <c r="E35" s="173"/>
       <c r="F35" s="148" t="s">
         <v>746</v>
       </c>
@@ -4210,25 +4210,25 @@
       <c r="J35" s="147"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="171"/>
-      <c r="B36" s="171"/>
-      <c r="C36" s="181"/>
-      <c r="D36" s="184"/>
-      <c r="E36" s="184"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="177"/>
+      <c r="C36" s="192"/>
+      <c r="D36" s="174"/>
+      <c r="E36" s="174"/>
       <c r="F36" s="150" t="s">
         <v>747</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="171"/>
-      <c r="B37" s="171"/>
-      <c r="C37" s="193" t="s">
+      <c r="A37" s="177"/>
+      <c r="B37" s="177"/>
+      <c r="C37" s="172" t="s">
         <v>728</v>
       </c>
-      <c r="D37" s="182" t="s">
+      <c r="D37" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="182" t="s">
+      <c r="E37" s="175" t="s">
         <v>714</v>
       </c>
       <c r="F37" s="148" t="s">
@@ -4236,141 +4236,141 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="171"/>
-      <c r="B38" s="171"/>
-      <c r="C38" s="183"/>
-      <c r="D38" s="183"/>
-      <c r="E38" s="183"/>
+      <c r="A38" s="177"/>
+      <c r="B38" s="177"/>
+      <c r="C38" s="173"/>
+      <c r="D38" s="173"/>
+      <c r="E38" s="173"/>
       <c r="F38" s="126" t="s">
         <v>749</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="172"/>
-      <c r="B39" s="172"/>
-      <c r="C39" s="184"/>
-      <c r="D39" s="184"/>
-      <c r="E39" s="184"/>
+      <c r="A39" s="178"/>
+      <c r="B39" s="178"/>
+      <c r="C39" s="174"/>
+      <c r="D39" s="174"/>
+      <c r="E39" s="174"/>
       <c r="F39" s="126" t="s">
         <v>750</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="170" t="s">
-        <v>772</v>
-      </c>
-      <c r="B40" s="185" t="s">
+      <c r="A40" s="176" t="s">
+        <v>771</v>
+      </c>
+      <c r="B40" s="182" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="187" t="s">
+      <c r="C40" s="184" t="s">
+        <v>780</v>
+      </c>
+      <c r="D40" s="188" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="188" t="s">
+        <v>782</v>
+      </c>
+      <c r="F40" s="151" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="177"/>
+      <c r="B41" s="183"/>
+      <c r="C41" s="185"/>
+      <c r="D41" s="189"/>
+      <c r="E41" s="189"/>
+      <c r="F41" s="158" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="177"/>
+      <c r="B42" s="183"/>
+      <c r="C42" s="185"/>
+      <c r="D42" s="189"/>
+      <c r="E42" s="189"/>
+      <c r="F42" s="158" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="177"/>
+      <c r="B43" s="183"/>
+      <c r="C43" s="186"/>
+      <c r="D43" s="186"/>
+      <c r="E43" s="186"/>
+      <c r="F43" s="134" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="177"/>
+      <c r="B44" s="183"/>
+      <c r="C44" s="186"/>
+      <c r="D44" s="186"/>
+      <c r="E44" s="186"/>
+      <c r="F44" s="134" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="177"/>
+      <c r="B45" s="183"/>
+      <c r="C45" s="186"/>
+      <c r="D45" s="186"/>
+      <c r="E45" s="186"/>
+      <c r="F45" s="134" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="177"/>
+      <c r="B46" s="183"/>
+      <c r="C46" s="186"/>
+      <c r="D46" s="186"/>
+      <c r="E46" s="186"/>
+      <c r="F46" s="134" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="177"/>
+      <c r="B47" s="183"/>
+      <c r="C47" s="187"/>
+      <c r="D47" s="187"/>
+      <c r="E47" s="187"/>
+      <c r="F47" s="135" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="177"/>
+      <c r="B48" s="177"/>
+      <c r="C48" s="152" t="s">
         <v>781</v>
-      </c>
-      <c r="D40" s="191" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="191" t="s">
-        <v>783</v>
-      </c>
-      <c r="F40" s="151" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="171"/>
-      <c r="B41" s="186"/>
-      <c r="C41" s="188"/>
-      <c r="D41" s="192"/>
-      <c r="E41" s="192"/>
-      <c r="F41" s="158" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="171"/>
-      <c r="B42" s="186"/>
-      <c r="C42" s="188"/>
-      <c r="D42" s="192"/>
-      <c r="E42" s="192"/>
-      <c r="F42" s="158" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="171"/>
-      <c r="B43" s="186"/>
-      <c r="C43" s="189"/>
-      <c r="D43" s="189"/>
-      <c r="E43" s="189"/>
-      <c r="F43" s="134" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="171"/>
-      <c r="B44" s="186"/>
-      <c r="C44" s="189"/>
-      <c r="D44" s="189"/>
-      <c r="E44" s="189"/>
-      <c r="F44" s="134" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="171"/>
-      <c r="B45" s="186"/>
-      <c r="C45" s="189"/>
-      <c r="D45" s="189"/>
-      <c r="E45" s="189"/>
-      <c r="F45" s="134" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="171"/>
-      <c r="B46" s="186"/>
-      <c r="C46" s="189"/>
-      <c r="D46" s="189"/>
-      <c r="E46" s="189"/>
-      <c r="F46" s="134" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="171"/>
-      <c r="B47" s="186"/>
-      <c r="C47" s="190"/>
-      <c r="D47" s="190"/>
-      <c r="E47" s="190"/>
-      <c r="F47" s="135" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="171"/>
-      <c r="B48" s="171"/>
-      <c r="C48" s="152" t="s">
-        <v>782</v>
       </c>
       <c r="D48" s="133" t="s">
         <v>9</v>
       </c>
       <c r="E48" s="133" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F48" s="137" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="171"/>
-      <c r="B49" s="171"/>
-      <c r="C49" s="193" t="s">
+      <c r="A49" s="177"/>
+      <c r="B49" s="177"/>
+      <c r="C49" s="172" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="182" t="s">
+      <c r="D49" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="182" t="s">
+      <c r="E49" s="175" t="s">
         <v>714</v>
       </c>
       <c r="F49" s="148" t="s">
@@ -4378,11 +4378,11 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="171"/>
-      <c r="B50" s="171"/>
-      <c r="C50" s="183"/>
-      <c r="D50" s="183"/>
-      <c r="E50" s="183"/>
+      <c r="A50" s="177"/>
+      <c r="B50" s="177"/>
+      <c r="C50" s="173"/>
+      <c r="D50" s="173"/>
+      <c r="E50" s="173"/>
       <c r="F50" s="126" t="s">
         <v>752</v>
       </c>
@@ -4391,28 +4391,28 @@
       <c r="I50" s="147"/>
     </row>
     <row r="51" spans="1:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="171"/>
-      <c r="B51" s="171"/>
-      <c r="C51" s="184"/>
-      <c r="D51" s="184"/>
-      <c r="E51" s="184"/>
+      <c r="A51" s="177"/>
+      <c r="B51" s="177"/>
+      <c r="C51" s="174"/>
+      <c r="D51" s="174"/>
+      <c r="E51" s="174"/>
       <c r="F51" s="127" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G51" s="149"/>
       <c r="H51" s="147"/>
       <c r="I51" s="147"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="171"/>
-      <c r="B52" s="171"/>
-      <c r="C52" s="179" t="s">
+      <c r="A52" s="177"/>
+      <c r="B52" s="177"/>
+      <c r="C52" s="190" t="s">
         <v>753</v>
       </c>
-      <c r="D52" s="182" t="s">
+      <c r="D52" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="E52" s="182" t="s">
+      <c r="E52" s="175" t="s">
         <v>717</v>
       </c>
       <c r="F52" s="148" t="s">
@@ -4420,11 +4420,11 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="171"/>
-      <c r="B53" s="171"/>
-      <c r="C53" s="180"/>
-      <c r="D53" s="183"/>
-      <c r="E53" s="183"/>
+      <c r="A53" s="177"/>
+      <c r="B53" s="177"/>
+      <c r="C53" s="191"/>
+      <c r="D53" s="173"/>
+      <c r="E53" s="173"/>
       <c r="F53" s="148" t="s">
         <v>755</v>
       </c>
@@ -4435,38 +4435,38 @@
       <c r="K53" s="147"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="171"/>
-      <c r="B54" s="171"/>
-      <c r="C54" s="180"/>
-      <c r="D54" s="183"/>
-      <c r="E54" s="183"/>
+      <c r="A54" s="177"/>
+      <c r="B54" s="177"/>
+      <c r="C54" s="191"/>
+      <c r="D54" s="173"/>
+      <c r="E54" s="173"/>
       <c r="F54" s="148" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="171"/>
-      <c r="B55" s="171"/>
-      <c r="C55" s="180"/>
-      <c r="D55" s="183"/>
-      <c r="E55" s="183"/>
+      <c r="A55" s="177"/>
+      <c r="B55" s="177"/>
+      <c r="C55" s="191"/>
+      <c r="D55" s="173"/>
+      <c r="E55" s="173"/>
       <c r="F55" s="148" t="s">
         <v>757</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="171"/>
-      <c r="B56" s="171"/>
-      <c r="C56" s="181"/>
-      <c r="D56" s="184"/>
-      <c r="E56" s="184"/>
+      <c r="A56" s="177"/>
+      <c r="B56" s="177"/>
+      <c r="C56" s="192"/>
+      <c r="D56" s="174"/>
+      <c r="E56" s="174"/>
       <c r="F56" s="150" t="s">
         <v>758</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="171"/>
-      <c r="B57" s="171"/>
+      <c r="A57" s="177"/>
+      <c r="B57" s="177"/>
       <c r="C57" s="144" t="s">
         <v>113</v>
       </c>
@@ -4477,35 +4477,35 @@
         <v>738</v>
       </c>
       <c r="F57" s="155" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="G57" s="140"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="171"/>
-      <c r="B58" s="171"/>
-      <c r="C58" s="197"/>
-      <c r="D58" s="183"/>
-      <c r="E58" s="199"/>
+      <c r="A58" s="177"/>
+      <c r="B58" s="177"/>
+      <c r="C58" s="193"/>
+      <c r="D58" s="173"/>
+      <c r="E58" s="170"/>
       <c r="F58" s="163" t="s">
+        <v>789</v>
+      </c>
+      <c r="G58" s="160"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="177"/>
+      <c r="B59" s="177"/>
+      <c r="C59" s="194"/>
+      <c r="D59" s="174"/>
+      <c r="E59" s="171"/>
+      <c r="F59" s="164" t="s">
         <v>790</v>
       </c>
-      <c r="G58" s="160"/>
-    </row>
-    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="171"/>
-      <c r="B59" s="171"/>
-      <c r="C59" s="198"/>
-      <c r="D59" s="184"/>
-      <c r="E59" s="200"/>
-      <c r="F59" s="164" t="s">
-        <v>791</v>
-      </c>
       <c r="G59" s="160"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="171"/>
-      <c r="B60" s="171"/>
+      <c r="A60" s="177"/>
+      <c r="B60" s="177"/>
       <c r="C60" s="162" t="s">
         <v>116</v>
       </c>
@@ -4516,37 +4516,37 @@
         <v>738</v>
       </c>
       <c r="F60" s="126" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G60" s="160"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="171"/>
-      <c r="B61" s="171"/>
+      <c r="A61" s="177"/>
+      <c r="B61" s="177"/>
       <c r="C61" s="162"/>
       <c r="D61" s="126"/>
       <c r="E61" s="126"/>
       <c r="F61" s="165" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G61" s="160"/>
     </row>
     <row r="62" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="171"/>
-      <c r="B62" s="171"/>
+      <c r="A62" s="177"/>
+      <c r="B62" s="177"/>
       <c r="C62" s="162"/>
       <c r="D62" s="126"/>
       <c r="E62" s="126"/>
       <c r="F62" s="165" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G62" s="160"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="171"/>
-      <c r="B63" s="171"/>
+      <c r="A63" s="177"/>
+      <c r="B63" s="177"/>
       <c r="C63" s="143" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D63" s="139" t="s">
         <v>13</v>
@@ -4555,37 +4555,37 @@
         <v>738</v>
       </c>
       <c r="F63" s="139" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G63" s="160"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="171"/>
-      <c r="B64" s="171"/>
+      <c r="A64" s="177"/>
+      <c r="B64" s="177"/>
       <c r="C64" s="145"/>
       <c r="D64" s="156"/>
       <c r="E64" s="156"/>
       <c r="F64" s="167" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G64" s="160"/>
     </row>
     <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="171"/>
-      <c r="B65" s="171"/>
+      <c r="A65" s="177"/>
+      <c r="B65" s="177"/>
       <c r="C65" s="146"/>
       <c r="D65" s="157"/>
       <c r="E65" s="126"/>
       <c r="F65" s="166" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G65" s="160"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="171"/>
-      <c r="B66" s="171"/>
+      <c r="A66" s="177"/>
+      <c r="B66" s="177"/>
       <c r="C66" s="144" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D66" s="155" t="s">
         <v>13</v>
@@ -4594,37 +4594,37 @@
         <v>738</v>
       </c>
       <c r="F66" s="139" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G66" s="160"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="171"/>
-      <c r="B67" s="171"/>
+      <c r="A67" s="177"/>
+      <c r="B67" s="177"/>
       <c r="C67" s="162"/>
       <c r="D67" s="126"/>
       <c r="E67" s="156"/>
       <c r="F67" s="167" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="G67" s="160"/>
     </row>
     <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="171"/>
-      <c r="B68" s="171"/>
+      <c r="A68" s="177"/>
+      <c r="B68" s="177"/>
       <c r="C68" s="146"/>
       <c r="D68" s="157"/>
       <c r="E68" s="157"/>
       <c r="F68" s="166" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G68" s="160"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="171"/>
-      <c r="B69" s="171"/>
+      <c r="A69" s="177"/>
+      <c r="B69" s="177"/>
       <c r="C69" s="144" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D69" s="139" t="s">
         <v>13</v>
@@ -4633,51 +4633,51 @@
         <v>738</v>
       </c>
       <c r="F69" s="139" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="G69" s="160"/>
     </row>
     <row r="70" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="171"/>
-      <c r="B70" s="171"/>
+      <c r="A70" s="177"/>
+      <c r="B70" s="177"/>
       <c r="C70" s="162"/>
       <c r="D70" s="156"/>
       <c r="E70" s="156"/>
       <c r="F70" s="167" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G70" s="160"/>
     </row>
     <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="171"/>
-      <c r="B71" s="171"/>
+      <c r="A71" s="177"/>
+      <c r="B71" s="177"/>
       <c r="C71" s="146"/>
       <c r="D71" s="157"/>
       <c r="E71" s="157"/>
       <c r="F71" s="166" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G71" s="160"/>
     </row>
     <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="171"/>
-      <c r="B72" s="171"/>
+      <c r="A72" s="177"/>
+      <c r="B72" s="177"/>
       <c r="C72" s="132" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D72" s="127" t="s">
         <v>9</v>
       </c>
       <c r="E72" s="127" t="s">
-        <v>759</v>
+        <v>818</v>
       </c>
       <c r="F72" s="127" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="171"/>
-      <c r="B73" s="171"/>
+      <c r="A73" s="177"/>
+      <c r="B73" s="177"/>
       <c r="C73" s="153" t="s">
         <v>737</v>
       </c>
@@ -4686,12 +4686,12 @@
       </c>
       <c r="E73" s="126"/>
       <c r="F73" s="126" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="171"/>
-      <c r="B74" s="171"/>
+      <c r="A74" s="177"/>
+      <c r="B74" s="177"/>
       <c r="C74" s="153"/>
       <c r="D74" s="126"/>
       <c r="E74" s="126"/>
@@ -4700,8 +4700,8 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="171"/>
-      <c r="B75" s="171"/>
+      <c r="A75" s="177"/>
+      <c r="B75" s="177"/>
       <c r="C75" s="153"/>
       <c r="D75" s="126"/>
       <c r="E75" s="126"/>
@@ -4710,47 +4710,47 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="171"/>
-      <c r="B76" s="171"/>
-      <c r="C76" s="193" t="s">
+      <c r="A76" s="177"/>
+      <c r="B76" s="177"/>
+      <c r="C76" s="172" t="s">
         <v>728</v>
       </c>
-      <c r="D76" s="182" t="s">
+      <c r="D76" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="E76" s="182" t="s">
+      <c r="E76" s="175" t="s">
         <v>714</v>
       </c>
       <c r="F76" s="126" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G76" s="159"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="171"/>
-      <c r="B77" s="171"/>
-      <c r="C77" s="183"/>
-      <c r="D77" s="183"/>
-      <c r="E77" s="183"/>
+      <c r="A77" s="177"/>
+      <c r="B77" s="177"/>
+      <c r="C77" s="173"/>
+      <c r="D77" s="173"/>
+      <c r="E77" s="173"/>
       <c r="F77" s="126" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="172"/>
-      <c r="B78" s="172"/>
-      <c r="C78" s="184"/>
-      <c r="D78" s="184"/>
-      <c r="E78" s="184"/>
+      <c r="A78" s="178"/>
+      <c r="B78" s="178"/>
+      <c r="C78" s="174"/>
+      <c r="D78" s="174"/>
+      <c r="E78" s="174"/>
       <c r="F78" s="127" t="s">
         <v>715</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="170" t="s">
-        <v>773</v>
-      </c>
-      <c r="B79" s="170" t="s">
+      <c r="A79" s="176" t="s">
+        <v>772</v>
+      </c>
+      <c r="B79" s="176" t="s">
         <v>718</v>
       </c>
       <c r="C79" s="131" t="s">
@@ -4767,72 +4767,72 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="171"/>
-      <c r="B80" s="171"/>
-      <c r="C80" s="173" t="s">
+      <c r="A80" s="177"/>
+      <c r="B80" s="177"/>
+      <c r="C80" s="195" t="s">
         <v>730</v>
       </c>
-      <c r="D80" s="176" t="s">
+      <c r="D80" s="198" t="s">
         <v>13</v>
       </c>
-      <c r="E80" s="176" t="s">
+      <c r="E80" s="198" t="s">
         <v>717</v>
       </c>
       <c r="F80" s="148" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="171"/>
-      <c r="B81" s="171"/>
-      <c r="C81" s="174"/>
-      <c r="D81" s="177"/>
-      <c r="E81" s="177"/>
+      <c r="A81" s="177"/>
+      <c r="B81" s="177"/>
+      <c r="C81" s="196"/>
+      <c r="D81" s="199"/>
+      <c r="E81" s="199"/>
       <c r="F81" s="154" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="G81" s="147"/>
       <c r="H81" s="147"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="171"/>
-      <c r="B82" s="171"/>
-      <c r="C82" s="174"/>
-      <c r="D82" s="177"/>
-      <c r="E82" s="177"/>
+      <c r="A82" s="177"/>
+      <c r="B82" s="177"/>
+      <c r="C82" s="196"/>
+      <c r="D82" s="199"/>
+      <c r="E82" s="199"/>
       <c r="F82" s="148" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G82" s="147"/>
       <c r="H82" s="147"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="171"/>
-      <c r="B83" s="171"/>
-      <c r="C83" s="174"/>
-      <c r="D83" s="177"/>
-      <c r="E83" s="177"/>
+      <c r="A83" s="177"/>
+      <c r="B83" s="177"/>
+      <c r="C83" s="196"/>
+      <c r="D83" s="199"/>
+      <c r="E83" s="199"/>
       <c r="F83" s="148" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G83" s="147"/>
       <c r="H83" s="147"/>
     </row>
     <row r="84" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="171"/>
-      <c r="B84" s="171"/>
-      <c r="C84" s="175"/>
-      <c r="D84" s="178"/>
-      <c r="E84" s="178"/>
+      <c r="A84" s="177"/>
+      <c r="B84" s="177"/>
+      <c r="C84" s="197"/>
+      <c r="D84" s="200"/>
+      <c r="E84" s="200"/>
       <c r="F84" s="150" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G84" s="147"/>
       <c r="H84" s="147"/>
     </row>
     <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="172"/>
-      <c r="B85" s="172"/>
+      <c r="A85" s="178"/>
+      <c r="B85" s="178"/>
       <c r="C85" s="132" t="s">
         <v>732</v>
       </c>
@@ -4872,6 +4872,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="A79:A85"/>
+    <mergeCell ref="B79:B85"/>
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="D80:D84"/>
+    <mergeCell ref="E80:E84"/>
+    <mergeCell ref="A16:A39"/>
+    <mergeCell ref="B16:B39"/>
+    <mergeCell ref="C32:C36"/>
+    <mergeCell ref="D32:D36"/>
+    <mergeCell ref="E32:E36"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="C52:C56"/>
+    <mergeCell ref="D52:D56"/>
+    <mergeCell ref="E52:E56"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="D76:D78"/>
+    <mergeCell ref="E76:E78"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="D58:D59"/>
     <mergeCell ref="E58:E59"/>
     <mergeCell ref="C37:C39"/>
     <mergeCell ref="D37:D39"/>
@@ -4888,28 +4910,6 @@
     <mergeCell ref="E40:E47"/>
     <mergeCell ref="C49:C51"/>
     <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="C52:C56"/>
-    <mergeCell ref="D52:D56"/>
-    <mergeCell ref="E52:E56"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="D76:D78"/>
-    <mergeCell ref="E76:E78"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="A16:A39"/>
-    <mergeCell ref="B16:B39"/>
-    <mergeCell ref="C32:C36"/>
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="E32:E36"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="A79:A85"/>
-    <mergeCell ref="B79:B85"/>
-    <mergeCell ref="C80:C84"/>
-    <mergeCell ref="D80:D84"/>
-    <mergeCell ref="E80:E84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -19659,21 +19659,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19697,14 +19697,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90F41780-9094-4F4A-BE43-209970D09E33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5536D9E3-D332-4E90-BF7B-48E6B0DB3F0F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -19720,4 +19712,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90F41780-9094-4F4A-BE43-209970D09E33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>